<commit_message>
finished some weather fetching and made a logistic regression model that only uses time and location info for predictions.
</commit_message>
<xml_diff>
--- a/Jeremy Thesis/Location Info Only Tests.xlsx
+++ b/Jeremy Thesis/Location Info Only Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Jeremy Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457C7A5A-6021-4F75-94F7-D21E41530D69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD1F0FB-1BAD-4333-A328-5A5C58C662A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
   <si>
     <t>Train_Acc</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>TS 50-50 TC</t>
+  </si>
+  <si>
+    <t>TS 50-50 TD</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
   </si>
 </sst>
 </file>
@@ -232,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +433,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -654,7 +672,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -678,6 +696,14 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1033,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,14 +1077,17 @@
     <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1106,7 +1135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -1138,26 +1167,25 @@
         <v>12466</v>
       </c>
       <c r="K2" s="6">
-        <v>0.81</v>
+        <v>81</v>
       </c>
       <c r="L2" s="6">
-        <v>0.81</v>
+        <v>81</v>
       </c>
       <c r="M2" s="6">
-        <v>0.82</v>
+        <v>82</v>
       </c>
       <c r="N2" s="6">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="O2" s="17">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="P2" s="7">
-        <f>2*((M2*L2)/(M2+L2))</f>
-        <v>0.81496932515337428</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>81.496932515337434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1189,26 +1217,25 @@
         <v>12393</v>
       </c>
       <c r="K3" s="19">
-        <v>0.78</v>
+        <v>78</v>
       </c>
       <c r="L3" s="19">
-        <v>0.77</v>
+        <v>77</v>
       </c>
       <c r="M3" s="19">
-        <v>0.82</v>
+        <v>82</v>
       </c>
       <c r="N3" s="19">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="O3" s="20">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="P3" s="4">
-        <f>2*((M3*L3)/(M3+L3))</f>
-        <v>0.79421383647798749</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>79.421383647798748</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>19</v>
       </c>
@@ -1240,30 +1267,80 @@
         <v>12428.7</v>
       </c>
       <c r="K4" s="15">
-        <v>0.79371571906354466</v>
+        <v>79.371571906354461</v>
       </c>
       <c r="L4" s="15">
-        <v>0.79284984987538465</v>
+        <v>79.284984987538465</v>
       </c>
       <c r="M4" s="15">
-        <v>0.8097400482116095</v>
+        <v>80.974004821160946</v>
       </c>
       <c r="N4" s="15">
-        <v>0.77681259019998572</v>
+        <v>77.681259019998578</v>
       </c>
       <c r="O4" s="15">
-        <v>0.2231874098000132</v>
+        <v>22.318740980001319</v>
       </c>
       <c r="P4" s="15">
-        <v>0.80119634577008347</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>80.119634577008341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="25">
+        <v>74.784634709358173</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0.17007550197726912</v>
+      </c>
+      <c r="D5" s="25">
+        <v>74.311036789297617</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0.17041288297658919</v>
+      </c>
+      <c r="F5" s="25">
+        <v>0.74264098171330417</v>
+      </c>
+      <c r="G5" s="27">
+        <v>10550.8</v>
+      </c>
+      <c r="H5" s="27">
+        <v>4038.2</v>
+      </c>
+      <c r="I5" s="27">
+        <v>3642.8</v>
+      </c>
+      <c r="J5" s="27">
+        <v>11668.2</v>
+      </c>
+      <c r="K5" s="25">
+        <v>74.311036789297617</v>
+      </c>
+      <c r="L5" s="25">
+        <v>74.280004066993982</v>
+      </c>
+      <c r="M5" s="25">
+        <v>76.207955064985924</v>
+      </c>
+      <c r="N5" s="25">
+        <v>72.32024127767491</v>
+      </c>
+      <c r="O5" s="25">
+        <v>27.679758722324987</v>
+      </c>
+      <c r="P5" s="25">
+        <v>75.219737345451662</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -1291,8 +1368,36 @@
       <c r="I8" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J8" s="26"/>
+      <c r="K8" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>43831</v>
       </c>
@@ -1320,8 +1425,35 @@
       <c r="I9" s="7">
         <v>8.2324455205811145</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K9" s="24">
+        <v>43831</v>
+      </c>
+      <c r="L9" s="23">
+        <v>13</v>
+      </c>
+      <c r="M9" s="23">
+        <v>52</v>
+      </c>
+      <c r="N9" s="23">
+        <v>3250</v>
+      </c>
+      <c r="O9" s="23">
+        <v>627</v>
+      </c>
+      <c r="P9" s="25">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="25">
+        <v>83.827701831312794</v>
+      </c>
+      <c r="R9" s="25">
+        <v>2.03125</v>
+      </c>
+      <c r="S9" s="25">
+        <v>3.6879432624113395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>43832</v>
       </c>
@@ -1349,8 +1481,35 @@
       <c r="I10" s="7">
         <v>15.514333895446878</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K10" s="24">
+        <v>43832</v>
+      </c>
+      <c r="L10" s="23">
+        <v>41</v>
+      </c>
+      <c r="M10" s="23">
+        <v>52</v>
+      </c>
+      <c r="N10" s="23">
+        <v>3262</v>
+      </c>
+      <c r="O10" s="23">
+        <v>1244</v>
+      </c>
+      <c r="P10" s="25">
+        <v>44.086021505376301</v>
+      </c>
+      <c r="Q10" s="25">
+        <v>72.392365734576103</v>
+      </c>
+      <c r="R10" s="25">
+        <v>3.1906614785992202</v>
+      </c>
+      <c r="S10" s="25">
+        <v>5.9506531204644402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>43833</v>
       </c>
@@ -1378,8 +1537,35 @@
       <c r="I11" s="7">
         <v>21.079046424090329</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K11" s="24">
+        <v>43833</v>
+      </c>
+      <c r="L11" s="23">
+        <v>71</v>
+      </c>
+      <c r="M11" s="23">
+        <v>75</v>
+      </c>
+      <c r="N11" s="23">
+        <v>2567</v>
+      </c>
+      <c r="O11" s="23">
+        <v>1886</v>
+      </c>
+      <c r="P11" s="25">
+        <v>48.630136986301295</v>
+      </c>
+      <c r="Q11" s="25">
+        <v>57.646530428924301</v>
+      </c>
+      <c r="R11" s="25">
+        <v>3.62800204394481</v>
+      </c>
+      <c r="S11" s="25">
+        <v>6.7522586780789302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>43834</v>
       </c>
@@ -1407,8 +1593,35 @@
       <c r="I12" s="7">
         <v>7.8838174273858916</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K12" s="24">
+        <v>43834</v>
+      </c>
+      <c r="L12" s="23">
+        <v>18</v>
+      </c>
+      <c r="M12" s="23">
+        <v>40</v>
+      </c>
+      <c r="N12" s="23">
+        <v>3305</v>
+      </c>
+      <c r="O12" s="23">
+        <v>1236</v>
+      </c>
+      <c r="P12" s="25">
+        <v>31.034482758620602</v>
+      </c>
+      <c r="Q12" s="25">
+        <v>72.781325699185189</v>
+      </c>
+      <c r="R12" s="25">
+        <v>1.4354066985645901</v>
+      </c>
+      <c r="S12" s="25">
+        <v>2.74390243902439</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>43835</v>
       </c>
@@ -1436,8 +1649,35 @@
       <c r="I13" s="7">
         <v>8.7336244541484707</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K13" s="24">
+        <v>43835</v>
+      </c>
+      <c r="L13" s="23">
+        <v>14</v>
+      </c>
+      <c r="M13" s="23">
+        <v>25</v>
+      </c>
+      <c r="N13" s="23">
+        <v>4129</v>
+      </c>
+      <c r="O13" s="23">
+        <v>431</v>
+      </c>
+      <c r="P13" s="25">
+        <v>35.897435897435898</v>
+      </c>
+      <c r="Q13" s="25">
+        <v>90.548245614034997</v>
+      </c>
+      <c r="R13" s="25">
+        <v>3.1460674157303306</v>
+      </c>
+      <c r="S13" s="25">
+        <v>5.7851239669421402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>43836</v>
       </c>
@@ -1465,8 +1705,35 @@
       <c r="I14" s="7">
         <v>12.229299363057324</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K14" s="24">
+        <v>43836</v>
+      </c>
+      <c r="L14" s="23">
+        <v>30</v>
+      </c>
+      <c r="M14" s="23">
+        <v>47</v>
+      </c>
+      <c r="N14" s="23">
+        <v>3943</v>
+      </c>
+      <c r="O14" s="23">
+        <v>579</v>
+      </c>
+      <c r="P14" s="25">
+        <v>38.961038961038902</v>
+      </c>
+      <c r="Q14" s="25">
+        <v>87.195931003980505</v>
+      </c>
+      <c r="R14" s="25">
+        <v>4.9261083743842295</v>
+      </c>
+      <c r="S14" s="25">
+        <v>8.7463556851311886</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>43837</v>
       </c>
@@ -1494,8 +1761,35 @@
       <c r="I15" s="7">
         <v>12.631578947368419</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K15" s="24">
+        <v>43837</v>
+      </c>
+      <c r="L15" s="23">
+        <v>37</v>
+      </c>
+      <c r="M15" s="23">
+        <v>68</v>
+      </c>
+      <c r="N15" s="23">
+        <v>3892</v>
+      </c>
+      <c r="O15" s="23">
+        <v>602</v>
+      </c>
+      <c r="P15" s="25">
+        <v>35.238095238095198</v>
+      </c>
+      <c r="Q15" s="25">
+        <v>86.604361370716504</v>
+      </c>
+      <c r="R15" s="25">
+        <v>5.7902973395931099</v>
+      </c>
+      <c r="S15" s="25">
+        <v>9.9462365591397806</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>16</v>
       </c>
@@ -1531,8 +1825,43 @@
         <f>AVERAGE(I9:I15)</f>
         <v>12.329163718868347</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="10">
+        <f>AVERAGE(L9:L15)</f>
+        <v>32</v>
+      </c>
+      <c r="M16" s="11">
+        <f t="shared" ref="M16:S16" si="1">AVERAGE(M9:M15)</f>
+        <v>51.285714285714285</v>
+      </c>
+      <c r="N16" s="11">
+        <f t="shared" si="1"/>
+        <v>3478.2857142857142</v>
+      </c>
+      <c r="O16" s="11">
+        <f t="shared" si="1"/>
+        <v>943.57142857142856</v>
+      </c>
+      <c r="P16" s="12">
+        <f t="shared" si="1"/>
+        <v>36.263887335266887</v>
+      </c>
+      <c r="Q16" s="12">
+        <f t="shared" si="1"/>
+        <v>78.713780240390051</v>
+      </c>
+      <c r="R16" s="12">
+        <f t="shared" si="1"/>
+        <v>3.4496847644023272</v>
+      </c>
+      <c r="S16" s="12">
+        <f t="shared" si="1"/>
+        <v>6.2303533873131727</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1560,8 +1889,36 @@
       <c r="I18" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="26"/>
+      <c r="K18" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43831</v>
       </c>
@@ -1589,8 +1946,35 @@
       <c r="I19" s="4">
         <v>7.3050345508390917</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K19" s="28">
+        <v>43831</v>
+      </c>
+      <c r="L19" s="29">
+        <v>31</v>
+      </c>
+      <c r="M19" s="29">
+        <v>34</v>
+      </c>
+      <c r="N19" s="29">
+        <v>3278</v>
+      </c>
+      <c r="O19" s="29">
+        <v>599</v>
+      </c>
+      <c r="P19" s="30">
+        <v>47.692307692307601</v>
+      </c>
+      <c r="Q19" s="30">
+        <v>84.549909724013389</v>
+      </c>
+      <c r="R19" s="30">
+        <v>4.92063492063492</v>
+      </c>
+      <c r="S19" s="30">
+        <v>8.9208633093525105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43832</v>
       </c>
@@ -1618,8 +2002,35 @@
       <c r="I20" s="4">
         <v>11.466165413533833</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20" s="28">
+        <v>43832</v>
+      </c>
+      <c r="L20" s="29">
+        <v>64</v>
+      </c>
+      <c r="M20" s="29">
+        <v>29</v>
+      </c>
+      <c r="N20" s="29">
+        <v>3841</v>
+      </c>
+      <c r="O20" s="29">
+        <v>665</v>
+      </c>
+      <c r="P20" s="30">
+        <v>68.817204301075193</v>
+      </c>
+      <c r="Q20" s="30">
+        <v>85.241899689303096</v>
+      </c>
+      <c r="R20" s="30">
+        <v>8.7791495198902592</v>
+      </c>
+      <c r="S20" s="30">
+        <v>15.571776155717702</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43833</v>
       </c>
@@ -1647,8 +2058,35 @@
       <c r="I21" s="4">
         <v>19.158460161145925</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="28">
+        <v>43833</v>
+      </c>
+      <c r="L21" s="29">
+        <v>98</v>
+      </c>
+      <c r="M21" s="29">
+        <v>48</v>
+      </c>
+      <c r="N21" s="29">
+        <v>3822</v>
+      </c>
+      <c r="O21" s="29">
+        <v>631</v>
+      </c>
+      <c r="P21" s="30">
+        <v>67.123287671232802</v>
+      </c>
+      <c r="Q21" s="30">
+        <v>85.829777677969901</v>
+      </c>
+      <c r="R21" s="30">
+        <v>13.443072702331902</v>
+      </c>
+      <c r="S21" s="30">
+        <v>22.400000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43834</v>
       </c>
@@ -1676,8 +2114,35 @@
       <c r="I22" s="4">
         <v>7.5801749271137027</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K22" s="28">
+        <v>43834</v>
+      </c>
+      <c r="L22" s="29">
+        <v>38</v>
+      </c>
+      <c r="M22" s="29">
+        <v>20</v>
+      </c>
+      <c r="N22" s="29">
+        <v>3850</v>
+      </c>
+      <c r="O22" s="29">
+        <v>691</v>
+      </c>
+      <c r="P22" s="30">
+        <v>65.517241379310292</v>
+      </c>
+      <c r="Q22" s="30">
+        <v>84.783087425677095</v>
+      </c>
+      <c r="R22" s="30">
+        <v>5.2126200274348404</v>
+      </c>
+      <c r="S22" s="30">
+        <v>9.6569250317661997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43835</v>
       </c>
@@ -1705,8 +2170,35 @@
       <c r="I23" s="4">
         <v>6.7326732673267333</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K23" s="28">
+        <v>43835</v>
+      </c>
+      <c r="L23" s="29">
+        <v>32</v>
+      </c>
+      <c r="M23" s="29">
+        <v>7</v>
+      </c>
+      <c r="N23" s="29">
+        <v>3863</v>
+      </c>
+      <c r="O23" s="29">
+        <v>697</v>
+      </c>
+      <c r="P23" s="30">
+        <v>82.051282051282001</v>
+      </c>
+      <c r="Q23" s="30">
+        <v>84.714912280701711</v>
+      </c>
+      <c r="R23" s="30">
+        <v>4.3895747599451296</v>
+      </c>
+      <c r="S23" s="30">
+        <v>8.3333333333333304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43836</v>
       </c>
@@ -1734,8 +2226,35 @@
       <c r="I24" s="4">
         <v>11.83206106870229</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K24" s="28">
+        <v>43836</v>
+      </c>
+      <c r="L24" s="29">
+        <v>58</v>
+      </c>
+      <c r="M24" s="29">
+        <v>19</v>
+      </c>
+      <c r="N24" s="29">
+        <v>3851</v>
+      </c>
+      <c r="O24" s="29">
+        <v>671</v>
+      </c>
+      <c r="P24" s="30">
+        <v>75.324675324675312</v>
+      </c>
+      <c r="Q24" s="30">
+        <v>85.161432994250291</v>
+      </c>
+      <c r="R24" s="30">
+        <v>7.9561042524005394</v>
+      </c>
+      <c r="S24" s="30">
+        <v>14.392059553349801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43837</v>
       </c>
@@ -1763,8 +2282,35 @@
       <c r="I25" s="4">
         <v>12.825278810408921</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K25" s="28">
+        <v>43837</v>
+      </c>
+      <c r="L25" s="29">
+        <v>59</v>
+      </c>
+      <c r="M25" s="29">
+        <v>46</v>
+      </c>
+      <c r="N25" s="29">
+        <v>3824</v>
+      </c>
+      <c r="O25" s="29">
+        <v>670</v>
+      </c>
+      <c r="P25" s="30">
+        <v>56.190476190476105</v>
+      </c>
+      <c r="Q25" s="30">
+        <v>85.091232754784102</v>
+      </c>
+      <c r="R25" s="30">
+        <v>8.0932784636488293</v>
+      </c>
+      <c r="S25" s="30">
+        <v>14.148681055155802</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>16</v>
       </c>
@@ -1773,23 +2319,23 @@
         <v>58.428571428571431</v>
       </c>
       <c r="C26" s="11">
-        <f t="shared" ref="C26:G26" si="1">AVERAGE(C19:C25)</f>
+        <f t="shared" ref="C26:G26" si="2">AVERAGE(C19:C25)</f>
         <v>24.857142857142858</v>
       </c>
       <c r="D26" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3512.5714285714284</v>
       </c>
       <c r="E26" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>909.28571428571433</v>
       </c>
       <c r="F26" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70.922396961287717</v>
       </c>
       <c r="G26" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>79.379887869837347</v>
       </c>
       <c r="H26" s="22">
@@ -1800,8 +2346,43 @@
         <f>AVERAGE(I19:I25)</f>
         <v>10.985692599867212</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="11">
+        <f>AVERAGE(L19:L25)</f>
+        <v>54.285714285714285</v>
+      </c>
+      <c r="M26" s="11">
+        <f t="shared" ref="M26:S26" si="3">AVERAGE(M19:M25)</f>
+        <v>29</v>
+      </c>
+      <c r="N26" s="11">
+        <f t="shared" si="3"/>
+        <v>3761.2857142857142</v>
+      </c>
+      <c r="O26" s="11">
+        <f t="shared" si="3"/>
+        <v>660.57142857142856</v>
+      </c>
+      <c r="P26" s="12">
+        <f t="shared" si="3"/>
+        <v>66.102353515765614</v>
+      </c>
+      <c r="Q26" s="12">
+        <f t="shared" si="3"/>
+        <v>85.053178935242798</v>
+      </c>
+      <c r="R26" s="12">
+        <f t="shared" si="3"/>
+        <v>7.5420620923266313</v>
+      </c>
+      <c r="S26" s="12">
+        <f t="shared" si="3"/>
+        <v>13.346234062667907</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>19</v>
       </c>
@@ -1829,8 +2410,9 @@
       <c r="I28" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>43831</v>
       </c>
@@ -1859,7 +2441,7 @@
         <v>3.68509212730318</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>43832</v>
       </c>
@@ -1888,7 +2470,7 @@
         <v>9.0395480225988702</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>43833</v>
       </c>
@@ -1917,7 +2499,7 @@
         <v>12.6816380449141</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>43834</v>
       </c>
@@ -1946,7 +2528,7 @@
         <v>4.1604754829123296</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>43835</v>
       </c>
@@ -1975,7 +2557,7 @@
         <v>3.3639143730886798</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>43836</v>
       </c>
@@ -2004,7 +2586,7 @@
         <v>7.8147612156295203</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>43837</v>
       </c>
@@ -2033,7 +2615,7 @@
         <v>6.9444444444444402</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>16</v>
       </c>
@@ -2042,33 +2624,36 @@
         <v>24</v>
       </c>
       <c r="C36" s="11">
-        <f t="shared" ref="C36:I36" si="2">AVERAGE(C29:C35)</f>
+        <f t="shared" ref="C36:I36" si="4">AVERAGE(C29:C35)</f>
         <v>58.571428571428569</v>
       </c>
       <c r="D36" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3720</v>
       </c>
       <c r="E36" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>579.14285714285711</v>
       </c>
       <c r="F36" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28.11619925909017</v>
       </c>
       <c r="G36" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>86.522823107627701</v>
       </c>
       <c r="H36" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.9423034939264503</v>
       </c>
       <c r="I36" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.8128391015558742</v>
       </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J38" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made a method that matches predictions based on distance
</commit_message>
<xml_diff>
--- a/Jeremy Thesis/Location Info Only Tests.xlsx
+++ b/Jeremy Thesis/Location Info Only Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Jeremy Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD1F0FB-1BAD-4333-A328-5A5C58C662A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96FBCED-1B14-4689-8548-21A7A0A8B2B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="27">
   <si>
     <t>Train_Acc</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>All variables available with ExtraTreesClassifier applied</t>
+  </si>
+  <si>
+    <t>The top 7 variables from above test</t>
+  </si>
+  <si>
+    <t>No weather</t>
+  </si>
+  <si>
+    <t>No location info (besides Grid_Num)</t>
+  </si>
+  <si>
+    <t>Grid_Num, Hour, DayFrame, Join Count</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1077,7 @@
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,6 +2426,12 @@
         <v>18</v>
       </c>
       <c r="J28" s="26"/>
+      <c r="K28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="16" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
@@ -2440,6 +2461,12 @@
       <c r="I29" s="15">
         <v>3.68509212730318</v>
       </c>
+      <c r="K29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L29" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
@@ -2469,6 +2496,12 @@
       <c r="I30" s="15">
         <v>9.0395480225988702</v>
       </c>
+      <c r="K30" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
@@ -2498,6 +2531,12 @@
       <c r="I31" s="15">
         <v>12.6816380449141</v>
       </c>
+      <c r="K31" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
@@ -2526,6 +2565,12 @@
       </c>
       <c r="I32" s="15">
         <v>4.1604754829123296</v>
+      </c>
+      <c r="K32" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Redid forecasting and remade the graphs showing the forecast results for January using the top 5 best performing models. Also, altered the methods that match predictions to their accidents so now it creates a nicely formatted file
</commit_message>
<xml_diff>
--- a/Jeremy Thesis/Location Info Only Tests.xlsx
+++ b/Jeremy Thesis/Location Info Only Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Jeremy Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96FBCED-1B14-4689-8548-21A7A0A8B2B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F6BCBD-D0F3-437D-A400-18EB96CCA802}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="28">
   <si>
     <t>Train_Acc</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Grid_Num, Hour, DayFrame, Join Count</t>
+  </si>
+  <si>
+    <t>MinWeath</t>
   </si>
 </sst>
 </file>
@@ -253,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,8 +466,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -642,6 +651,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -687,7 +705,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -719,6 +737,10 @@
     <xf numFmtId="14" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -766,6 +788,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFD256C3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1074,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,7 +2726,274 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J38" s="26"/>
+      <c r="A38" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" s="31"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="33">
+        <v>43831</v>
+      </c>
+      <c r="B39" s="32">
+        <v>16</v>
+      </c>
+      <c r="C39" s="32">
+        <v>49</v>
+      </c>
+      <c r="D39" s="32">
+        <v>3001</v>
+      </c>
+      <c r="E39" s="32">
+        <v>768</v>
+      </c>
+      <c r="F39" s="34">
+        <v>24.615384615384599</v>
+      </c>
+      <c r="G39" s="34">
+        <v>79.623242239320703</v>
+      </c>
+      <c r="H39" s="34">
+        <v>2.0408163265306101</v>
+      </c>
+      <c r="I39" s="34">
+        <v>3.7691401648998797</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="33">
+        <v>43832</v>
+      </c>
+      <c r="B40" s="32">
+        <v>41</v>
+      </c>
+      <c r="C40" s="32">
+        <v>52</v>
+      </c>
+      <c r="D40" s="32">
+        <v>3461</v>
+      </c>
+      <c r="E40" s="32">
+        <v>919</v>
+      </c>
+      <c r="F40" s="34">
+        <v>44.086021505376301</v>
+      </c>
+      <c r="G40" s="34">
+        <v>79.018264840182596</v>
+      </c>
+      <c r="H40" s="34">
+        <v>4.2708333333333304</v>
+      </c>
+      <c r="I40" s="34">
+        <v>7.7872744539411203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="33">
+        <v>43833</v>
+      </c>
+      <c r="B41" s="32">
+        <v>51</v>
+      </c>
+      <c r="C41" s="32">
+        <v>91</v>
+      </c>
+      <c r="D41" s="32">
+        <v>3575</v>
+      </c>
+      <c r="E41" s="32">
+        <v>756</v>
+      </c>
+      <c r="F41" s="34">
+        <v>35.915492957746395</v>
+      </c>
+      <c r="G41" s="34">
+        <v>82.544447009928405</v>
+      </c>
+      <c r="H41" s="34">
+        <v>6.3197026022304801</v>
+      </c>
+      <c r="I41" s="34">
+        <v>10.748155953635399</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="33">
+        <v>43834</v>
+      </c>
+      <c r="B42" s="32">
+        <v>21</v>
+      </c>
+      <c r="C42" s="32">
+        <v>37</v>
+      </c>
+      <c r="D42" s="32">
+        <v>3485</v>
+      </c>
+      <c r="E42" s="32">
+        <v>930</v>
+      </c>
+      <c r="F42" s="34">
+        <v>36.2068965517241</v>
+      </c>
+      <c r="G42" s="34">
+        <v>78.935447338618303</v>
+      </c>
+      <c r="H42" s="34">
+        <v>2.2082018927444698</v>
+      </c>
+      <c r="I42" s="34">
+        <v>4.1625371655104004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="33">
+        <v>43835</v>
+      </c>
+      <c r="B43" s="32">
+        <v>12</v>
+      </c>
+      <c r="C43" s="32">
+        <v>27</v>
+      </c>
+      <c r="D43" s="32">
+        <v>3463</v>
+      </c>
+      <c r="E43" s="32">
+        <v>971</v>
+      </c>
+      <c r="F43" s="34">
+        <v>30.769230769230699</v>
+      </c>
+      <c r="G43" s="34">
+        <v>78.101037437979201</v>
+      </c>
+      <c r="H43" s="34">
+        <v>1.22075279755849</v>
+      </c>
+      <c r="I43" s="34">
+        <v>2.3483365949119301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="33">
+        <v>43836</v>
+      </c>
+      <c r="B44" s="32">
+        <v>30</v>
+      </c>
+      <c r="C44" s="32">
+        <v>46</v>
+      </c>
+      <c r="D44" s="32">
+        <v>3703</v>
+      </c>
+      <c r="E44" s="32">
+        <v>694</v>
+      </c>
+      <c r="F44" s="34">
+        <v>39.473684210526301</v>
+      </c>
+      <c r="G44" s="34">
+        <v>84.216511257675592</v>
+      </c>
+      <c r="H44" s="34">
+        <v>4.1436464088397695</v>
+      </c>
+      <c r="I44" s="34">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="33">
+        <v>43837</v>
+      </c>
+      <c r="B45" s="32">
+        <v>34</v>
+      </c>
+      <c r="C45" s="32">
+        <v>71</v>
+      </c>
+      <c r="D45" s="32">
+        <v>3454</v>
+      </c>
+      <c r="E45" s="32">
+        <v>914</v>
+      </c>
+      <c r="F45" s="34">
+        <v>32.380952380952301</v>
+      </c>
+      <c r="G45" s="34">
+        <v>79.075091575091506</v>
+      </c>
+      <c r="H45" s="34">
+        <v>3.5864978902953504</v>
+      </c>
+      <c r="I45" s="34">
+        <v>6.4577397910731191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="11">
+        <f>AVERAGE(B39:B45)</f>
+        <v>29.285714285714285</v>
+      </c>
+      <c r="C46" s="11">
+        <f t="shared" ref="C46:I46" si="5">AVERAGE(C39:C45)</f>
+        <v>53.285714285714285</v>
+      </c>
+      <c r="D46" s="11">
+        <f t="shared" si="5"/>
+        <v>3448.8571428571427</v>
+      </c>
+      <c r="E46" s="11">
+        <f t="shared" si="5"/>
+        <v>850.28571428571433</v>
+      </c>
+      <c r="F46" s="12">
+        <f t="shared" si="5"/>
+        <v>34.778237570134387</v>
+      </c>
+      <c r="G46" s="12">
+        <f t="shared" si="5"/>
+        <v>80.216291671256613</v>
+      </c>
+      <c r="H46" s="12">
+        <f t="shared" si="5"/>
+        <v>3.3986358930760714</v>
+      </c>
+      <c r="I46" s="12">
+        <f t="shared" si="5"/>
+        <v>6.1104548748531213</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>